<commit_message>
Fix setup data upload and import
</commit_message>
<xml_diff>
--- a/src/bika/lims/setupdata/test/test.xlsx
+++ b/src/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="58"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -712,10 +712,10 @@
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">Lab administartion and accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micro-Biological analysis</t>
+    <t xml:space="preserve">Lab administration and accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbiological analysis</t>
   </si>
   <si>
     <t xml:space="preserve">Test</t>
@@ -763,7 +763,7 @@
     <t xml:space="preserve">Rare Specimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Exremely rare specimen for control purposes</t>
+    <t xml:space="preserve">Extremely rare specimen for Control purposes</t>
   </si>
   <si>
     <t xml:space="preserve">Bag</t>
@@ -868,7 +868,7 @@
     <t xml:space="preserve">021 555 3417</t>
   </si>
   <si>
-    <t xml:space="preserve">mwf@example.com</t>
+    <t xml:space="preserve">myrtle@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Ruff</t>
@@ -949,7 +949,7 @@
     <t xml:space="preserve">082 607 8405</t>
   </si>
   <si>
-    <t xml:space="preserve">mohale@example.com</t>
+    <t xml:space="preserve">happy_mohale@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Ŝarel Seemonster</t>
@@ -982,7 +982,7 @@
     <t xml:space="preserve">083 644 8576</t>
   </si>
   <si>
-    <t xml:space="preserve">seemonster@example.com</t>
+    <t xml:space="preserve">happy_seemonster@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Rita Mohale</t>
@@ -1015,7 +1015,7 @@
     <t xml:space="preserve">080 564 7509</t>
   </si>
   <si>
-    <t xml:space="preserve">standard@example.com</t>
+    <t xml:space="preserve">happy_standard@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Ŝarel Seemonster, Rita Mohale</t>
@@ -1048,7 +1048,7 @@
     <t xml:space="preserve">081 569 7909</t>
   </si>
   <si>
-    <t xml:space="preserve">smith@example.com</t>
+    <t xml:space="preserve">klaymore_smith@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Fred</t>
@@ -1078,7 +1078,7 @@
     <t xml:space="preserve">084 677 8884</t>
   </si>
   <si>
-    <t xml:space="preserve">turner@example.com</t>
+    <t xml:space="preserve">myrtle_fredturner@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Chris</t>
@@ -1105,7 +1105,7 @@
     <t xml:space="preserve">074 304 5021</t>
   </si>
   <si>
-    <t xml:space="preserve">ruffian@example.com</t>
+    <t xml:space="preserve">ruff_ruffian@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Andre</t>
@@ -1135,7 +1135,7 @@
     <t xml:space="preserve">078 469 7035</t>
   </si>
   <si>
-    <t xml:space="preserve">corbin@example.com</t>
+    <t xml:space="preserve">sunnyside_corbin@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Attachment Types</t>
@@ -5780,7 +5780,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5850,7 +5850,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6375,7 +6375,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6554,7 +6554,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7327,7 +7327,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8097,8 +8097,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12016,7 +12016,7 @@
   <dimension ref="A1:Y89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18331,7 +18331,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25681,7 +25681,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27053,7 +27053,7 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -27473,7 +27473,7 @@
   <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29199,8 +29199,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29213,7 +29213,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="15" style="0" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="9.13"/>
@@ -29829,7 +29829,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29896,7 +29896,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O60" activeCellId="0" sqref="O60"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>